<commit_message>
update secret key for excel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Staff.xlsx
+++ b/src/main/resources/templates/excel/Staff.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SmartWay\SmartWay-SEP490\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA31735B-444B-46D8-9831-1EB766C9C750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82586D95-8585-4717-B36A-1E680C9CFEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="LmGGT9+g2jJaZ7F9X0GETwByiIOUA0hNBhWLdQ9b3o1NPqy4fQymCFyZ9IRxSC8/eCk0iYTiO2ayRo+z13Ks3Q==" workbookSaltValue="uUG1mEAOkY5tv8rLT28E3A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="228" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff-Manage" sheetId="1" r:id="rId1"/>
+    <sheet name="Secret_Key" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -417,7 +419,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,4 +455,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD480A8-DD21-4EE3-9EC8-46652C4FA9A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Y0tZ68DiWc1aj2PpElBc/WhwoD+yKLYPLZa1i3p9n4Gusng1eylWyNF31sNtZeTxv1BxR6rEi+ENRBu5RhlAJA==" saltValue="uRF9/0ZsChzvr98URncBGA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last update of import staff
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/Staff.xlsx
+++ b/src/main/resources/templates/excel/Staff.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SmartWay\SmartWay-SEP490\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82586D95-8585-4717-B36A-1E680C9CFEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECE0CAE-5BBD-4BFD-93AB-59673B01BA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="LmGGT9+g2jJaZ7F9X0GETwByiIOUA0hNBhWLdQ9b3o1NPqy4fQymCFyZ9IRxSC8/eCk0iYTiO2ayRo+z13Ks3Q==" workbookSaltValue="uUG1mEAOkY5tv8rLT28E3A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="228" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1248" yWindow="576" windowWidth="21624" windowHeight="11304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Staff-Manage" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,7 +75,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF4D81F1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -108,16 +115,23 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4D81F1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -419,41 +433,43 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="vUdcOgp6NdgBQlMJgvPm7Cey42NxMvHNkNL0FzH9S90l9lhd/qY+UUmw5CWXapxerlbYH8G3Vm76DnBxA+RD/g==" saltValue="B9djU86lnZf7QiJIVqyizw==" spinCount="100000" sheet="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>